<commit_message>
merubah seluruh database (excel dan table)
</commit_message>
<xml_diff>
--- a/Flow Chart Simponi Universitas Jenny.xlsx
+++ b/Flow Chart Simponi Universitas Jenny.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kerja Jenny\Simponi Universitas Jenny\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\Desktop\Simponi-Universitas-Jenny\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C81549-DC83-4B6A-B734-FD70B6598D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8595190E-4FEC-40F4-9FD4-96D7DFA04172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{AD6234D6-FEE0-470F-94DC-DB0FB8CD84D0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="44">
   <si>
     <t>user_login</t>
   </si>
@@ -50,15 +50,9 @@
     <t>rule</t>
   </si>
   <si>
-    <t>user_identity</t>
-  </si>
-  <si>
     <t>int</t>
   </si>
   <si>
-    <t>name_user</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -107,21 +101,9 @@
     <t>task_file</t>
   </si>
   <si>
-    <t>file</t>
-  </si>
-  <si>
-    <t>task_details</t>
-  </si>
-  <si>
-    <t>task_id</t>
-  </si>
-  <si>
     <t>score</t>
   </si>
   <si>
-    <t>user_identity_id</t>
-  </si>
-  <si>
     <t>clock</t>
   </si>
   <si>
@@ -156,6 +138,33 @@
   </si>
   <si>
     <t>day</t>
+  </si>
+  <si>
+    <t>student_identity</t>
+  </si>
+  <si>
+    <t>lecturer_identity</t>
+  </si>
+  <si>
+    <t>nid</t>
+  </si>
+  <si>
+    <t>student_identity_id</t>
+  </si>
+  <si>
+    <t>lecturer_identity_id</t>
+  </si>
+  <si>
+    <t>daedline</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>blob</t>
+  </si>
+  <si>
+    <t>photo</t>
   </si>
 </sst>
 </file>
@@ -171,15 +180,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -213,16 +234,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C6121F9-40F6-4207-9BC5-94BDC0DCA3AC}">
-  <dimension ref="B3:L26"/>
+  <dimension ref="B3:L21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,139 +606,143 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="H3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="K3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L3" s="1"/>
+      <c r="C3" s="7"/>
+      <c r="E3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="H3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="7"/>
+      <c r="K3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="7"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>2</v>
+      <c r="E5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="I6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="7"/>
       <c r="E7" s="1" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K7" s="2" t="s">
+      <c r="H7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>6</v>
+      <c r="L7" s="5" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="K8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>2</v>
+      <c r="E8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
@@ -695,171 +753,247 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="1" t="s">
+      <c r="H10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="E12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" s="7"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="E15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="E16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H12" s="1" t="s">
+      <c r="L19" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="1"/>
-      <c r="H18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E21" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
+      <c r="L21" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
merubah sedikit table, memperbaiki tampilan untuk daftar mahasiswa, menambah layer membuat jadwal, dan berhasil mengkoneksi file library ke express.js
</commit_message>
<xml_diff>
--- a/Flow Chart Simponi Universitas Jenny.xlsx
+++ b/Flow Chart Simponi Universitas Jenny.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\Desktop\Simponi-Universitas-Jenny\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\Simponi-Universitas-Jenny\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8595190E-4FEC-40F4-9FD4-96D7DFA04172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302C99DA-79BF-4D65-9D07-5516C22D93CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{AD6234D6-FEE0-470F-94DC-DB0FB8CD84D0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="45">
   <si>
     <t>user_login</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>photo</t>
+  </si>
+  <si>
+    <t>major_last_education</t>
   </si>
 </sst>
 </file>
@@ -200,7 +203,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -221,17 +224,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -264,17 +256,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -591,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C6121F9-40F6-4207-9BC5-94BDC0DCA3AC}">
-  <dimension ref="B3:L21"/>
+  <dimension ref="B3:L19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,22 +596,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="E3" s="6" t="s">
+      <c r="C3" s="5"/>
+      <c r="E3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="H3" s="6" t="s">
+      <c r="F3" s="5"/>
+      <c r="H3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="K3" s="6" t="s">
+      <c r="I3" s="5"/>
+      <c r="K3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="7"/>
+      <c r="L3" s="5"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -656,22 +646,22 @@
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="5" t="s">
+      <c r="F5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="5" t="s">
+      <c r="I5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -688,18 +678,18 @@
       <c r="I6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="L6" s="5" t="s">
+      <c r="K6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="5"/>
       <c r="E7" s="1" t="s">
         <v>41</v>
       </c>
@@ -712,10 +702,10 @@
       <c r="I7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K7" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="L7" s="5" t="s">
+      <c r="K7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -738,11 +728,11 @@
       <c r="I8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K8" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>5</v>
+      <c r="K8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
@@ -764,18 +754,18 @@
       <c r="I9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>2</v>
+      <c r="K9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -789,12 +779,6 @@
       </c>
       <c r="I10" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
@@ -810,12 +794,16 @@
       <c r="I11" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="K11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L11" s="5"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="7"/>
+      <c r="C12" s="5"/>
       <c r="E12" s="1" t="s">
         <v>28</v>
       </c>
@@ -828,10 +816,12 @@
       <c r="I12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K12" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L12" s="7"/>
+      <c r="K12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
@@ -852,10 +842,10 @@
       <c r="I13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L13" s="1" t="s">
+      <c r="K13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L13" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -878,121 +868,115 @@
       <c r="I14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="K14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="L14" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="E15" s="4" t="s">
+      <c r="C15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I15" s="3" t="s">
+      <c r="F16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="E17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="L15" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="E16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L17" s="5" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="K19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="K20" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="K21" s="3" t="s">
+      <c r="C19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L21" s="3" t="s">
+      <c r="L19" s="2" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="K3:L3"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B3:C3"/>
+    <mergeCell ref="K11:L11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
menyelesaikan html untuk master (sampai menambah jadwal mata kuliah) dan memperbaiki tabel kembali
</commit_message>
<xml_diff>
--- a/Flow Chart Simponi Universitas Jenny.xlsx
+++ b/Flow Chart Simponi Universitas Jenny.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\Simponi-Universitas-Jenny\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\Desktop\Simponi-Universitas-Jenny\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302C99DA-79BF-4D65-9D07-5516C22D93CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB2AD75-2CBF-469A-80F0-B1F1FA234900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{AD6234D6-FEE0-470F-94DC-DB0FB8CD84D0}"/>
   </bookViews>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="46">
   <si>
     <t>user_login</t>
   </si>
@@ -149,9 +141,6 @@
     <t>nid</t>
   </si>
   <si>
-    <t>student_identity_id</t>
-  </si>
-  <si>
     <t>lecturer_identity_id</t>
   </si>
   <si>
@@ -168,6 +157,12 @@
   </si>
   <si>
     <t>major_last_education</t>
+  </si>
+  <si>
+    <t>major_name</t>
+  </si>
+  <si>
+    <t>major_id</t>
   </si>
 </sst>
 </file>
@@ -256,10 +251,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -267,6 +261,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C6121F9-40F6-4207-9BC5-94BDC0DCA3AC}">
-  <dimension ref="B3:L19"/>
+  <dimension ref="B3:L21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,22 +595,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="E3" s="4" t="s">
+      <c r="C3" s="4"/>
+      <c r="E3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="H3" s="4" t="s">
+      <c r="F3" s="4"/>
+      <c r="H3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="5"/>
-      <c r="K3" s="4" t="s">
+      <c r="I3" s="4"/>
+      <c r="K3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="5"/>
+      <c r="L3" s="4"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -646,22 +645,22 @@
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="3" t="s">
+      <c r="F5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L5" s="3" t="s">
+      <c r="I5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -678,35 +677,35 @@
       <c r="I6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" s="3" t="s">
+      <c r="K6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="4"/>
       <c r="E7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>5</v>
+      <c r="K7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
@@ -729,10 +728,10 @@
         <v>2</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
@@ -754,18 +753,14 @@
       <c r="I9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -794,16 +789,16 @@
       <c r="I11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L11" s="5"/>
+      <c r="L11" s="4"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="4"/>
       <c r="E12" s="1" t="s">
         <v>28</v>
       </c>
@@ -842,10 +837,10 @@
       <c r="I13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K13" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L13" s="3" t="s">
+      <c r="K13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L13" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -868,115 +863,140 @@
       <c r="I14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L14" s="3" t="s">
+      <c r="K14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L14" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="2" t="s">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="E15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="F15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K15" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>5</v>
+      <c r="I15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="4"/>
       <c r="E16" s="2" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="5"/>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="E17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="H17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="5"/>
       <c r="K17" s="1" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>24</v>
+      <c r="I18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L19" s="2" t="s">
+      <c r="H19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="2" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="K3:L3"/>
-    <mergeCell ref="B17:C17"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="K11:L11"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="B16:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
melanjutkan membuat frontend (sampai mahasiswa - daftar tugas - belum selesai) dan memperbaiki database kembali
</commit_message>
<xml_diff>
--- a/Flow Chart Simponi Universitas Jenny.xlsx
+++ b/Flow Chart Simponi Universitas Jenny.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\Desktop\Simponi-Universitas-Jenny\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB2AD75-2CBF-469A-80F0-B1F1FA234900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91EB559-0840-42E6-95FB-699457A21A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{AD6234D6-FEE0-470F-94DC-DB0FB8CD84D0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="50">
   <si>
     <t>user_login</t>
   </si>
@@ -84,9 +84,6 @@
     <t>material_name</t>
   </si>
   <si>
-    <t>task</t>
-  </si>
-  <si>
     <t>task_name</t>
   </si>
   <si>
@@ -163,6 +160,21 @@
   </si>
   <si>
     <t>major_id</t>
+  </si>
+  <si>
+    <t>student_identity_id</t>
+  </si>
+  <si>
+    <t>task_lecturer</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>task_student</t>
+  </si>
+  <si>
+    <t>task_lecturer_id</t>
   </si>
 </sst>
 </file>
@@ -198,7 +210,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -247,11 +259,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -261,11 +295,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,423 +617,453 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C6121F9-40F6-4207-9BC5-94BDC0DCA3AC}">
-  <dimension ref="B3:L21"/>
+  <dimension ref="B1:L21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="27.85546875" customWidth="1"/>
     <col min="5" max="5" width="27.85546875" customWidth="1"/>
     <col min="8" max="8" width="27.85546875" customWidth="1"/>
     <col min="11" max="11" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="E1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="H1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="4"/>
+      <c r="K1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="4"/>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="E3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="4"/>
-      <c r="H3" s="3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="4"/>
-      <c r="K3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3" s="4"/>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="I4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="E5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="L9" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="E10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="1" t="s">
+      <c r="C11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="E14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K4" s="1" t="s">
+      <c r="C15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="4"/>
+      <c r="K15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="E7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L11" s="4"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="E12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="E15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="E16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>2</v>
+      <c r="I16" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>21</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="L18" s="8"/>
+    </row>
+    <row r="19" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I17" s="5"/>
-      <c r="K17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="H19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="H20" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="H21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>5</v>
+      <c r="L19" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="K20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="K21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="B16:C16"/>
+  <mergeCells count="10">
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="K8:L8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
menyelesaikan frontend dan memperbaiki database kembali untuk yang kesekian kalinya :')
</commit_message>
<xml_diff>
--- a/Flow Chart Simponi Universitas Jenny.xlsx
+++ b/Flow Chart Simponi Universitas Jenny.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\Desktop\Simponi-Universitas-Jenny\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91EB559-0840-42E6-95FB-699457A21A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6452EE9-3E9A-4B35-AB51-B9E0C309BC6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{AD6234D6-FEE0-470F-94DC-DB0FB8CD84D0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="50">
   <si>
     <t>user_login</t>
   </si>
@@ -210,7 +210,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -281,28 +281,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -617,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C6121F9-40F6-4207-9BC5-94BDC0DCA3AC}">
-  <dimension ref="B1:L21"/>
+  <dimension ref="B1:L22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,22 +641,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="6"/>
+      <c r="E1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="H1" s="3" t="s">
+      <c r="F1" s="6"/>
+      <c r="H1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="K1" s="3" t="s">
+      <c r="I1" s="6"/>
+      <c r="K1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="4"/>
+      <c r="L1" s="6"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -723,10 +731,10 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="6"/>
       <c r="E5" s="1" t="s">
         <v>39</v>
       </c>
@@ -739,11 +747,11 @@
       <c r="I5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>2</v>
+      <c r="K5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
@@ -766,10 +774,10 @@
         <v>2</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
@@ -791,6 +799,12 @@
       <c r="I7" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="K7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
@@ -811,10 +825,6 @@
       <c r="I8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="L8" s="4"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E9" s="1" t="s">
@@ -829,18 +839,16 @@
       <c r="I9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="K9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="L9" s="6"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="6"/>
       <c r="E10" s="1" t="s">
         <v>27</v>
       </c>
@@ -853,10 +861,10 @@
       <c r="I10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L10" s="2" t="s">
+      <c r="K10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -880,7 +888,7 @@
         <v>2</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>5</v>
@@ -905,11 +913,11 @@
       <c r="I12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>2</v>
+      <c r="K12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
@@ -925,18 +933,18 @@
       <c r="I13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>2</v>
+      <c r="K13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="6"/>
       <c r="E14" s="2" t="s">
         <v>44</v>
       </c>
@@ -944,10 +952,10 @@
         <v>2</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>40</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
@@ -964,14 +972,14 @@
         <v>5</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="I15" s="4"/>
       <c r="K15" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
@@ -994,76 +1002,84 @@
         <v>5</v>
       </c>
       <c r="K16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="H17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="H18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H17" s="1" t="s">
+      <c r="L18" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H18" s="2" t="s">
+      <c r="F20" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E21" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K18" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="L18" s="8"/>
-    </row>
-    <row r="19" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H19" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="K20" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="K21" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L21" s="6" t="s">
-        <v>40</v>
-      </c>
+      <c r="F21" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="E1:F1"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="E1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
memperbaiki database untuk yg kesekian kalinya dan mengetest inputan mahasiswa
</commit_message>
<xml_diff>
--- a/Flow Chart Simponi Universitas Jenny.xlsx
+++ b/Flow Chart Simponi Universitas Jenny.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\Desktop\Simponi-Universitas-Jenny\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\Simponi-Universitas-Jenny\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6452EE9-3E9A-4B35-AB51-B9E0C309BC6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8120CCE6-1AD4-4CC0-A8C1-9AC5BD6600F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{AD6234D6-FEE0-470F-94DC-DB0FB8CD84D0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="51">
   <si>
     <t>user_login</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>task_lecturer_id</t>
+  </si>
+  <si>
+    <t>study_program</t>
   </si>
 </sst>
 </file>
@@ -210,7 +213,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -281,36 +284,26 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,7 +621,7 @@
   <dimension ref="B1:L22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,22 +634,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="E1" s="5" t="s">
+      <c r="C1" s="4"/>
+      <c r="E1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="H1" s="5" t="s">
+      <c r="F1" s="4"/>
+      <c r="H1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="K1" s="5" t="s">
+      <c r="I1" s="4"/>
+      <c r="K1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="6"/>
+      <c r="L1" s="4"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -731,10 +724,10 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="4"/>
       <c r="E5" s="1" t="s">
         <v>39</v>
       </c>
@@ -839,16 +832,16 @@
       <c r="I9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="L9" s="6"/>
+      <c r="L9" s="4"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="4"/>
       <c r="E10" s="1" t="s">
         <v>27</v>
       </c>
@@ -941,10 +934,10 @@
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="6"/>
+      <c r="C14" s="4"/>
       <c r="E14" s="2" t="s">
         <v>44</v>
       </c>
@@ -966,15 +959,15 @@
         <v>5</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I15" s="4"/>
+      <c r="I15" s="6"/>
       <c r="K15" s="1" t="s">
         <v>47</v>
       </c>
@@ -990,10 +983,10 @@
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>1</v>
@@ -1009,6 +1002,12 @@
       </c>
     </row>
     <row r="17" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="H17" s="2" t="s">
         <v>49</v>
       </c>
@@ -1023,10 +1022,6 @@
       </c>
     </row>
     <row r="18" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E18" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="6"/>
       <c r="H18" s="1" t="s">
         <v>20</v>
       </c>
@@ -1041,45 +1036,47 @@
       </c>
     </row>
     <row r="19" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="E19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="4"/>
     </row>
     <row r="20" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
+      <c r="F22" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="E1:F1"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="K9:L9"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="E1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
selesai membuat layer, memperbaiki sisa kembali (1)
</commit_message>
<xml_diff>
--- a/Flow Chart Simponi Universitas Jenny.xlsx
+++ b/Flow Chart Simponi Universitas Jenny.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\Simponi-Universitas-Jenny\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\Desktop\Simponi-Universitas-Jenny\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8120CCE6-1AD4-4CC0-A8C1-9AC5BD6600F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD45F3B9-08AB-4A94-ACA7-7E7EC06EA401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{AD6234D6-FEE0-470F-94DC-DB0FB8CD84D0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="52">
   <si>
     <t>user_login</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>study_program</t>
+  </si>
+  <si>
+    <t>study_program_id</t>
   </si>
 </sst>
 </file>
@@ -288,20 +291,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -322,7 +330,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -610,7 +618,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -621,7 +629,7 @@
   <dimension ref="B1:L22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B10" sqref="B10:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,22 +642,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="6"/>
+      <c r="E1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="H1" s="3" t="s">
+      <c r="F1" s="6"/>
+      <c r="H1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="K1" s="3" t="s">
+      <c r="I1" s="6"/>
+      <c r="K1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="4"/>
+      <c r="L1" s="6"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -724,10 +732,10 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="6"/>
       <c r="E5" s="1" t="s">
         <v>39</v>
       </c>
@@ -832,16 +840,16 @@
       <c r="I9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="K9" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="L9" s="4"/>
+      <c r="L9" s="6"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="6"/>
       <c r="E10" s="1" t="s">
         <v>27</v>
       </c>
@@ -934,10 +942,10 @@
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="6"/>
       <c r="E14" s="2" t="s">
         <v>44</v>
       </c>
@@ -964,10 +972,10 @@
       <c r="F15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I15" s="6"/>
+      <c r="I15" s="4"/>
       <c r="K15" s="1" t="s">
         <v>47</v>
       </c>
@@ -976,11 +984,11 @@
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>2</v>
+      <c r="B16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>13</v>
@@ -1001,7 +1009,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="E17" s="1" t="s">
         <v>41</v>
       </c>
@@ -1021,7 +1035,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H18" s="1" t="s">
         <v>20</v>
       </c>
@@ -1035,13 +1049,23 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E19" s="3" t="s">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="E19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="4"/>
-    </row>
-    <row r="20" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="E20" s="1" t="s">
         <v>1</v>
       </c>
@@ -1049,7 +1073,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>2</v>
+      </c>
       <c r="E21" s="1" t="s">
         <v>16</v>
       </c>
@@ -1057,7 +1087,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
       <c r="E22" s="2" t="s">
         <v>45</v>
       </c>
@@ -1066,17 +1098,18 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="K9:L9"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="K9:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
memperbaiki sisa yang masih error (4)
</commit_message>
<xml_diff>
--- a/Flow Chart Simponi Universitas Jenny.xlsx
+++ b/Flow Chart Simponi Universitas Jenny.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\Desktop\Simponi-Universitas-Jenny\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B517A73-0BB9-4FE4-8036-669E1AA50367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F155A4-46BC-403C-A928-8AF9B95A745C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{AD6234D6-FEE0-470F-94DC-DB0FB8CD84D0}"/>
   </bookViews>
@@ -295,9 +295,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -308,6 +305,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -328,7 +328,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -627,7 +627,7 @@
   <dimension ref="B1:L21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,22 +640,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="E1" s="4" t="s">
+      <c r="C1" s="4"/>
+      <c r="E1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="H1" s="4" t="s">
+      <c r="F1" s="4"/>
+      <c r="H1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="5"/>
-      <c r="K1" s="4" t="s">
+      <c r="I1" s="4"/>
+      <c r="K1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="5"/>
+      <c r="L1" s="4"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -730,10 +730,10 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="4"/>
       <c r="E5" s="1" t="s">
         <v>39</v>
       </c>
@@ -838,16 +838,16 @@
       <c r="I9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="L9" s="5"/>
+      <c r="L9" s="4"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="4"/>
       <c r="E10" s="1" t="s">
         <v>27</v>
       </c>
@@ -950,7 +950,7 @@
         <v>44</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>41</v>
@@ -966,10 +966,10 @@
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="5"/>
+      <c r="C15" s="4"/>
       <c r="E15" s="1" t="s">
         <v>13</v>
       </c>
@@ -996,10 +996,10 @@
       <c r="F16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I16" s="7"/>
+      <c r="I16" s="6"/>
       <c r="K16" s="1" t="s">
         <v>20</v>
       </c>
@@ -1028,10 +1028,10 @@
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="5"/>
+      <c r="F18" s="4"/>
       <c r="H18" s="2" t="s">
         <v>49</v>
       </c>
@@ -1046,10 +1046,10 @@
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="3"/>
+      <c r="C19" s="7"/>
       <c r="E19" s="1" t="s">
         <v>1</v>
       </c>
@@ -1070,11 +1070,11 @@
       <c r="C20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>2</v>
+      <c r="E20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
@@ -1084,26 +1084,26 @@
       <c r="C21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>5</v>
+      <c r="E21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B1:C1"/>
     <mergeCell ref="K9:L9"/>
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E18:F18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
memperbaiki perubahan yang ada (5)
</commit_message>
<xml_diff>
--- a/Flow Chart Simponi Universitas Jenny.xlsx
+++ b/Flow Chart Simponi Universitas Jenny.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\Desktop\Simponi-Universitas-Jenny\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F155A4-46BC-403C-A928-8AF9B95A745C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1626E8-6AD2-4694-B222-69D60C256784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{AD6234D6-FEE0-470F-94DC-DB0FB8CD84D0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="51">
   <si>
     <t>user_login</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>semester</t>
-  </si>
-  <si>
-    <t>class_id</t>
   </si>
   <si>
     <t>class</t>
@@ -295,6 +292,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -305,9 +305,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -627,7 +624,7 @@
   <dimension ref="B1:L21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,22 +637,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="5"/>
+      <c r="E1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="H1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="H1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="4"/>
-      <c r="K1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L1" s="4"/>
+      <c r="I1" s="5"/>
+      <c r="K1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="5"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -685,7 +682,7 @@
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
@@ -703,7 +700,7 @@
         <v>2</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>5</v>
@@ -711,43 +708,43 @@
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>5</v>
+      <c r="L4" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="5"/>
       <c r="E5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>5</v>
@@ -761,19 +758,19 @@
         <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>2</v>
@@ -799,15 +796,15 @@
         <v>2</v>
       </c>
       <c r="K7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -827,35 +824,35 @@
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="L9" s="4"/>
+      <c r="K9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L9" s="5"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="5"/>
       <c r="E10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>2</v>
@@ -887,7 +884,7 @@
         <v>2</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>5</v>
@@ -895,51 +892,51 @@
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L12" s="2" t="s">
-        <v>5</v>
+      <c r="L12" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>5</v>
@@ -947,29 +944,29 @@
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E14" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="4"/>
+      <c r="B15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="5"/>
       <c r="E15" s="1" t="s">
         <v>13</v>
       </c>
@@ -977,7 +974,7 @@
         <v>5</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>2</v>
@@ -991,25 +988,25 @@
         <v>5</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="I16" s="6"/>
+        <v>39</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I16" s="7"/>
       <c r="K16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>2</v>
@@ -1021,35 +1018,35 @@
         <v>5</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="4"/>
+      <c r="E18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="5"/>
       <c r="H18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="7"/>
+      <c r="C19" s="3"/>
       <c r="E19" s="1" t="s">
         <v>1</v>
       </c>
@@ -1057,10 +1054,10 @@
         <v>5</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
@@ -1071,7 +1068,7 @@
         <v>5</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>5</v>
@@ -1079,13 +1076,13 @@
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>2</v>
@@ -1093,17 +1090,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="E1:F1"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E18:F18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
memperbaiki perubahan yang ada (6)
</commit_message>
<xml_diff>
--- a/Flow Chart Simponi Universitas Jenny.xlsx
+++ b/Flow Chart Simponi Universitas Jenny.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\Desktop\Simponi-Universitas-Jenny\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1626E8-6AD2-4694-B222-69D60C256784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9999075-38DA-4004-9CB9-DB825E6EF225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{AD6234D6-FEE0-470F-94DC-DB0FB8CD84D0}"/>
   </bookViews>
@@ -292,9 +292,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -305,6 +302,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -624,7 +624,7 @@
   <dimension ref="B1:L21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,22 +637,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="E1" s="4" t="s">
+      <c r="C1" s="4"/>
+      <c r="E1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="H1" s="4" t="s">
+      <c r="F1" s="4"/>
+      <c r="H1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="5"/>
-      <c r="K1" s="4" t="s">
+      <c r="I1" s="4"/>
+      <c r="K1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="5"/>
+      <c r="L1" s="4"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -720,17 +720,17 @@
         <v>5</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="4"/>
       <c r="E5" s="1" t="s">
         <v>38</v>
       </c>
@@ -835,16 +835,16 @@
       <c r="I9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="L9" s="5"/>
+      <c r="L9" s="4"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="4"/>
       <c r="E10" s="1" t="s">
         <v>26</v>
       </c>
@@ -910,7 +910,7 @@
         <v>2</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>2</v>
@@ -963,10 +963,10 @@
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="5"/>
+      <c r="C15" s="4"/>
       <c r="E15" s="1" t="s">
         <v>13</v>
       </c>
@@ -993,10 +993,10 @@
       <c r="F16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="I16" s="7"/>
+      <c r="I16" s="6"/>
       <c r="K16" s="1" t="s">
         <v>19</v>
       </c>
@@ -1025,10 +1025,10 @@
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="5"/>
+      <c r="F18" s="4"/>
       <c r="H18" s="2" t="s">
         <v>48</v>
       </c>
@@ -1043,10 +1043,10 @@
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="3"/>
+      <c r="C19" s="7"/>
       <c r="E19" s="1" t="s">
         <v>1</v>
       </c>
@@ -1090,17 +1090,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B1:C1"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="K9:L9"/>
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>